<commit_message>
Add production service form
</commit_message>
<xml_diff>
--- a/xlsforms/productionservice.xlsx
+++ b/xlsforms/productionservice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -39,12 +39,18 @@
     <t xml:space="preserve">constraint</t>
   </si>
   <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
     <t xml:space="preserve">string</t>
   </si>
   <si>
     <t xml:space="preserve">Name </t>
   </si>
   <si>
+    <t xml:space="preserve">select_one producer_types</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -117,6 +123,75 @@
     <t xml:space="preserve">GPS Accuracy</t>
   </si>
   <si>
+    <t xml:space="preserve">raw_material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source of raw material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water_quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water quantity need (in m³ per month)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energy_consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average energy consumption (in kWh per month)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storagepoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:ForeignKey("storagepoint.Storagepoint")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salepoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:ForeignKey("salepoint.Salepoint")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance: production site → storage → shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covid_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are the measures taken in the context of limiting COVID-19 infection affecting you?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one main_effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main_effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main effect is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turnover_decrease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the percentage by which you estimate the decrease in turnover?</t>
+  </si>
+  <si>
     <t xml:space="preserve">list name</t>
   </si>
   <si>
@@ -141,6 +216,126 @@
     <t xml:space="preserve">Enter Manually</t>
   </si>
   <si>
+    <t xml:space="preserve">producer_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificate of producer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small_company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small_gardening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small gardening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main_effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaderea_vanzarilor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scăderea vânzărilor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaderea_cifrei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scăderea cifrei de afaceri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disponibilizari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilizări</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intarzieri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Întârzieri la plata furnizorilor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dificultati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dificultăţi la încasare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restrangerea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restrângerea activității</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suspendarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspendarea temporară a activităţii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inchiderea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Închiderea firmei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reprofilare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reprofilare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 – 20 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20_40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 – 40 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 – 60 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 60 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
@@ -156,7 +351,7 @@
     <t xml:space="preserve">style</t>
   </si>
   <si>
-    <t xml:space="preserve">shop</t>
+    <t xml:space="preserve">productionservice</t>
   </si>
 </sst>
 </file>
@@ -318,15 +513,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,15 +618,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="31.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -453,7 +652,9 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
       <c r="AMH1" s="1"/>
@@ -462,179 +663,292 @@
     </row>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G5" s="4"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="AMJ6" s="9"/>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="AMJ7" s="9"/>
-    </row>
-    <row r="8" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="AMJ8" s="9"/>
-    </row>
-    <row r="9" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="AMJ9" s="9"/>
-    </row>
-    <row r="10" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G10" s="4"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0"/>
-    </row>
-    <row r="16" s="8" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0"/>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G16" s="4"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="AMJ23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="22.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="22.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+    </row>
     <row r="27" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="24.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -666,6 +980,10 @@
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -684,22 +1002,22 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="31.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="81.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="10" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
@@ -708,52 +1026,257 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="0"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -777,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,28 +1316,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="D2" s="13" t="n">
         <v>1</v>

</xml_diff>